<commit_message>
add new image product
</commit_message>
<xml_diff>
--- a/resources/imports/ProductCategorySeeder.xlsx
+++ b/resources/imports/ProductCategorySeeder.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dafid\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kampus\Perkuliahan\Semester 4\Pemrograman Web\Proyek Akhir\source\mlijo-apps\resources\imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A751DBEC-6637-43CE-A656-B08921304897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FA9819-5ED8-4136-9942-8BD58159D0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29925" yWindow="1125" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35715" yWindow="4005" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kategori Produk" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>No.</t>
   </si>
@@ -126,46 +126,43 @@
     <t>perlengkapan-makanan</t>
   </si>
   <si>
-    <t>buah_buahan.png</t>
-  </si>
-  <si>
-    <t>ayam_ayam.png</t>
-  </si>
-  <si>
-    <t>ikan_seafood.png</t>
-  </si>
-  <si>
-    <t>daging_daging.png</t>
-  </si>
-  <si>
-    <t>kesehatan_kesehatan.png</t>
-  </si>
-  <si>
-    <t>sayur_segar.png</t>
-  </si>
-  <si>
-    <t>jajanan_pasar.png</t>
-  </si>
-  <si>
-    <t>bumbu_kue.png</t>
-  </si>
-  <si>
-    <t>tahu_nabati.png</t>
-  </si>
-  <si>
-    <t>siap_olahan.png</t>
-  </si>
-  <si>
-    <t>kopi_minuman.png</t>
-  </si>
-  <si>
-    <t>susu_susu.png</t>
-  </si>
-  <si>
-    <t>rumah_tangga.png</t>
-  </si>
-  <si>
-    <t>perlengkapan_makanan.png</t>
+    <t>icon-11.png</t>
+  </si>
+  <si>
+    <t>icon-12.png</t>
+  </si>
+  <si>
+    <t>icon-10.png</t>
+  </si>
+  <si>
+    <t>icon-9.png</t>
+  </si>
+  <si>
+    <t>icon-14.png</t>
+  </si>
+  <si>
+    <t>icon-8.png</t>
+  </si>
+  <si>
+    <t>icon-6.png</t>
+  </si>
+  <si>
+    <t>icon-1.png</t>
+  </si>
+  <si>
+    <t>icon-4.png</t>
+  </si>
+  <si>
+    <t>icon-2.png</t>
+  </si>
+  <si>
+    <t>icon-13.png</t>
+  </si>
+  <si>
+    <t>icon-3.png</t>
+  </si>
+  <si>
+    <t>icon-5.png</t>
   </si>
 </sst>
 </file>
@@ -501,7 +498,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +549,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -566,7 +563,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -580,7 +577,7 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
@@ -594,7 +591,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -608,7 +605,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -622,7 +619,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -636,7 +633,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
         <v>26</v>
@@ -650,7 +647,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
         <v>27</v>
@@ -664,7 +661,7 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
         <v>28</v>
@@ -678,7 +675,7 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
         <v>29</v>
@@ -692,7 +689,7 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
         <v>30</v>
@@ -706,7 +703,7 @@
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
         <v>31</v>
@@ -720,7 +717,7 @@
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E15" t="s">
         <v>32</v>

</xml_diff>